<commit_message>
Cut excel to 50 rows
</commit_message>
<xml_diff>
--- a/public/SalesData.xlsx
+++ b/public/SalesData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>First Name</t>
   </si>
@@ -323,303 +323,6 @@
   </si>
   <si>
     <t>Stannering</t>
-  </si>
-  <si>
-    <t>Halley</t>
-  </si>
-  <si>
-    <t>Cricket</t>
-  </si>
-  <si>
-    <t>Babita</t>
-  </si>
-  <si>
-    <t>O' Molan</t>
-  </si>
-  <si>
-    <t>Torie</t>
-  </si>
-  <si>
-    <t>Hallwood</t>
-  </si>
-  <si>
-    <t>Gilberto</t>
-  </si>
-  <si>
-    <t>Lyon</t>
-  </si>
-  <si>
-    <t>Ofilia</t>
-  </si>
-  <si>
-    <t>Nozzolinii</t>
-  </si>
-  <si>
-    <t>Elladine</t>
-  </si>
-  <si>
-    <t>Darinton</t>
-  </si>
-  <si>
-    <t>Alister</t>
-  </si>
-  <si>
-    <t>De la croix</t>
-  </si>
-  <si>
-    <t>Allison</t>
-  </si>
-  <si>
-    <t>Vinnicombe</t>
-  </si>
-  <si>
-    <t>Ann</t>
-  </si>
-  <si>
-    <t>Swindells</t>
-  </si>
-  <si>
-    <t>Coop</t>
-  </si>
-  <si>
-    <t>Poulsom</t>
-  </si>
-  <si>
-    <t>Verine</t>
-  </si>
-  <si>
-    <t>Binnell</t>
-  </si>
-  <si>
-    <t>Claudius</t>
-  </si>
-  <si>
-    <t>Gannicott</t>
-  </si>
-  <si>
-    <t>Hagan</t>
-  </si>
-  <si>
-    <t>Risbridger</t>
-  </si>
-  <si>
-    <t>Baxie</t>
-  </si>
-  <si>
-    <t>Bordis</t>
-  </si>
-  <si>
-    <t>Lynnell</t>
-  </si>
-  <si>
-    <t>Braunton</t>
-  </si>
-  <si>
-    <t>Natka</t>
-  </si>
-  <si>
-    <t>Rahill</t>
-  </si>
-  <si>
-    <t>Leon</t>
-  </si>
-  <si>
-    <t>Wickes</t>
-  </si>
-  <si>
-    <t>Muffin</t>
-  </si>
-  <si>
-    <t>Egell</t>
-  </si>
-  <si>
-    <t>Dodie</t>
-  </si>
-  <si>
-    <t>Feary</t>
-  </si>
-  <si>
-    <t>Nickolas</t>
-  </si>
-  <si>
-    <t>Gooding</t>
-  </si>
-  <si>
-    <t>Emmey</t>
-  </si>
-  <si>
-    <t>Sibson</t>
-  </si>
-  <si>
-    <t>Tiff</t>
-  </si>
-  <si>
-    <t>Everly</t>
-  </si>
-  <si>
-    <t>Roosevelt</t>
-  </si>
-  <si>
-    <t>Townson</t>
-  </si>
-  <si>
-    <t>Denni</t>
-  </si>
-  <si>
-    <t>Scallan</t>
-  </si>
-  <si>
-    <t>Buddy</t>
-  </si>
-  <si>
-    <t>Brewins</t>
-  </si>
-  <si>
-    <t>Garey</t>
-  </si>
-  <si>
-    <t>Cavaney</t>
-  </si>
-  <si>
-    <t>Renata</t>
-  </si>
-  <si>
-    <t>Rugieri</t>
-  </si>
-  <si>
-    <t>Joella</t>
-  </si>
-  <si>
-    <t>Gouldthorpe</t>
-  </si>
-  <si>
-    <t>Merrill</t>
-  </si>
-  <si>
-    <t>Hendrickson</t>
-  </si>
-  <si>
-    <t>Abella</t>
-  </si>
-  <si>
-    <t>Waylon</t>
-  </si>
-  <si>
-    <t>Otham</t>
-  </si>
-  <si>
-    <t>Marylynne</t>
-  </si>
-  <si>
-    <t>Feathersby</t>
-  </si>
-  <si>
-    <t>Vernor</t>
-  </si>
-  <si>
-    <t>Lage</t>
-  </si>
-  <si>
-    <t>Shirlene</t>
-  </si>
-  <si>
-    <t>Golda</t>
-  </si>
-  <si>
-    <t>Joana</t>
-  </si>
-  <si>
-    <t>Pruce</t>
-  </si>
-  <si>
-    <t>Megan</t>
-  </si>
-  <si>
-    <t>Tompkin</t>
-  </si>
-  <si>
-    <t>Perice</t>
-  </si>
-  <si>
-    <t>Kobes</t>
-  </si>
-  <si>
-    <t>Merola</t>
-  </si>
-  <si>
-    <t>Daid</t>
-  </si>
-  <si>
-    <t>Tressa</t>
-  </si>
-  <si>
-    <t>Couch</t>
-  </si>
-  <si>
-    <t>Nathanael</t>
-  </si>
-  <si>
-    <t>Littell</t>
-  </si>
-  <si>
-    <t>Nerta</t>
-  </si>
-  <si>
-    <t>Helkin</t>
-  </si>
-  <si>
-    <t>Marge</t>
-  </si>
-  <si>
-    <t>Kynan</t>
-  </si>
-  <si>
-    <t>Rossie</t>
-  </si>
-  <si>
-    <t>McIlwrath</t>
-  </si>
-  <si>
-    <t>Isadore</t>
-  </si>
-  <si>
-    <t>Grasner</t>
-  </si>
-  <si>
-    <t>Judy</t>
-  </si>
-  <si>
-    <t>Commings</t>
-  </si>
-  <si>
-    <t>Burnaby</t>
-  </si>
-  <si>
-    <t>Duffer</t>
-  </si>
-  <si>
-    <t>Flemming</t>
-  </si>
-  <si>
-    <t>Fawley</t>
-  </si>
-  <si>
-    <t>Nanny</t>
-  </si>
-  <si>
-    <t>Giacomucci</t>
-  </si>
-  <si>
-    <t>Dane</t>
-  </si>
-  <si>
-    <t>Durnall</t>
-  </si>
-  <si>
-    <t>Pace</t>
-  </si>
-  <si>
-    <t>Hebbron</t>
   </si>
 </sst>
 </file>
@@ -641,9 +344,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="14"/>
       <color indexed="8"/>
-      <name val="Cambria"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="14"/>
@@ -651,7 +354,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,7 +369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -676,8 +379,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -700,26 +409,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -728,7 +499,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -750,125 +539,12 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff8064a2"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffe6e6e6"/>
       <rgbColor rgb="ffcacaca"/>
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>447641</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>49563</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>13334</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Shape 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7686641" y="4861560"/>
-          <a:ext cx="275023" cy="161925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill flip="none" rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="39B7D8"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent5">
-                <a:hueOff val="249502"/>
-                <a:satOff val="48101"/>
-                <a:lumOff val="28891"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat">
-          <a:solidFill>
-            <a:srgbClr val="46AAC4"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>574641</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>138430</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>258964</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Shape 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7813641" y="4988560"/>
-          <a:ext cx="357424" cy="215900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1003,13 +679,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1108,10 +778,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1366,13 +1036,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1685,10 +1349,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1939,17 +1603,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.1875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7812" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.4844" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.4688" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
@@ -1965,1412 +1630,816 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" ht="12.6" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>80193</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>30000</v>
       </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" ht="12.6" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="A3" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="10">
         <v>141182</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="10">
         <v>35000</v>
       </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" ht="12.6" customHeight="1">
-      <c r="A4" t="s" s="3">
+      <c r="A4" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="6">
         <v>61456</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>15000</v>
       </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" ht="12.6" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="A5" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="B5" t="s" s="5">
+      <c r="B5" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="10">
         <v>99354</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="10">
         <v>95000</v>
       </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" ht="12.6" customHeight="1">
-      <c r="A6" t="s" s="3">
+      <c r="A6" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B6" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="6">
         <v>139701</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>50000</v>
       </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" ht="12.6" customHeight="1">
-      <c r="A7" t="s" s="5">
+      <c r="A7" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="B7" t="s" s="5">
+      <c r="B7" t="s" s="9">
         <v>15</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="10">
         <v>63808</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>25000</v>
       </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" ht="12.6" customHeight="1">
-      <c r="A8" t="s" s="3">
+      <c r="A8" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B8" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="6">
         <v>50211</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <v>60000</v>
       </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" ht="12.6" customHeight="1">
-      <c r="A9" t="s" s="5">
+      <c r="A9" t="s" s="9">
         <v>18</v>
       </c>
-      <c r="B9" t="s" s="5">
+      <c r="B9" t="s" s="9">
         <v>19</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="10">
         <v>78556</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>35000</v>
       </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" ht="12.6" customHeight="1">
-      <c r="A10" t="s" s="3">
+      <c r="A10" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B10" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="6">
         <v>122695</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="6">
         <v>100000</v>
       </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" ht="12.6" customHeight="1">
-      <c r="A11" t="s" s="5">
+      <c r="A11" t="s" s="9">
         <v>22</v>
       </c>
-      <c r="B11" t="s" s="5">
+      <c r="B11" t="s" s="9">
         <v>23</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="10">
         <v>115410</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>70000</v>
       </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" ht="12.6" customHeight="1">
-      <c r="A12" t="s" s="3">
+      <c r="A12" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B12" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="6">
         <v>106991</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="6">
         <v>75000</v>
       </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" ht="12.6" customHeight="1">
-      <c r="A13" t="s" s="5">
+      <c r="A13" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="B13" t="s" s="5">
+      <c r="B13" t="s" s="9">
         <v>27</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="10">
         <v>25924</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="10">
         <v>85000</v>
       </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" ht="12.6" customHeight="1">
-      <c r="A14" t="s" s="3">
+      <c r="A14" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B14" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="6">
         <v>43564</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="6">
         <v>85000</v>
       </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" ht="12.6" customHeight="1">
-      <c r="A15" t="s" s="5">
+      <c r="A15" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B15" t="s" s="5">
+      <c r="B15" t="s" s="9">
         <v>31</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="10">
         <v>131725</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="10">
         <v>5000</v>
       </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" ht="12.6" customHeight="1">
-      <c r="A16" t="s" s="3">
+      <c r="A16" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B16" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="6">
         <v>100336</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="6">
         <v>35000</v>
       </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" ht="12.6" customHeight="1">
-      <c r="A17" t="s" s="5">
+      <c r="A17" t="s" s="9">
         <v>34</v>
       </c>
-      <c r="B17" t="s" s="5">
+      <c r="B17" t="s" s="9">
         <v>35</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="10">
         <v>143750</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="10">
         <v>100000</v>
       </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" ht="12.6" customHeight="1">
-      <c r="A18" t="s" s="3">
+      <c r="A18" t="s" s="5">
         <v>36</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B18" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="6">
         <v>22729</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="6">
         <v>10000</v>
       </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" ht="12.6" customHeight="1">
-      <c r="A19" t="s" s="5">
+      <c r="A19" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="B19" t="s" s="5">
+      <c r="B19" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="10">
         <v>140919</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="10">
         <v>10000</v>
       </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" ht="12.6" customHeight="1">
-      <c r="A20" t="s" s="3">
+      <c r="A20" t="s" s="5">
         <v>40</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B20" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="6">
         <v>70981</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="6">
         <v>10000</v>
       </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" ht="12.6" customHeight="1">
-      <c r="A21" t="s" s="5">
+      <c r="A21" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="B21" t="s" s="5">
+      <c r="B21" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="10">
         <v>80516</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="10">
         <v>10000</v>
       </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" ht="12.6" customHeight="1">
-      <c r="A22" t="s" s="3">
+      <c r="A22" t="s" s="5">
         <v>44</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B22" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="6">
         <v>118852</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="6">
         <v>65000</v>
       </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" ht="12.6" customHeight="1">
-      <c r="A23" t="s" s="5">
+      <c r="A23" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="B23" t="s" s="5">
+      <c r="B23" t="s" s="9">
         <v>47</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="10">
         <v>122953</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="10">
         <v>10000</v>
       </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" ht="12.6" customHeight="1">
-      <c r="A24" t="s" s="3">
+      <c r="A24" t="s" s="5">
         <v>48</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B24" t="s" s="5">
         <v>49</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="6">
         <v>46997</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="6">
         <v>45000</v>
       </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" ht="12.6" customHeight="1">
-      <c r="A25" t="s" s="5">
+      <c r="A25" t="s" s="9">
         <v>50</v>
       </c>
-      <c r="B25" t="s" s="5">
+      <c r="B25" t="s" s="9">
         <v>51</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="10">
         <v>91465</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="10">
         <v>100000</v>
       </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" ht="12.6" customHeight="1">
-      <c r="A26" t="s" s="3">
+      <c r="A26" t="s" s="5">
         <v>52</v>
       </c>
-      <c r="B26" t="s" s="3">
+      <c r="B26" t="s" s="5">
         <v>53</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="6">
         <v>66825</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="6">
         <v>60000</v>
       </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" ht="12.6" customHeight="1">
-      <c r="A27" t="s" s="5">
+      <c r="A27" t="s" s="9">
         <v>54</v>
       </c>
-      <c r="B27" t="s" s="5">
+      <c r="B27" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="10">
         <v>131244</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="10">
         <v>50000</v>
       </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" ht="12.6" customHeight="1">
-      <c r="A28" t="s" s="3">
+      <c r="A28" t="s" s="5">
         <v>56</v>
       </c>
-      <c r="B28" t="s" s="3">
+      <c r="B28" t="s" s="5">
         <v>57</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="6">
         <v>94131</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="6">
         <v>30000</v>
       </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" ht="12.6" customHeight="1">
-      <c r="A29" t="s" s="5">
+      <c r="A29" t="s" s="9">
         <v>58</v>
       </c>
-      <c r="B29" t="s" s="5">
+      <c r="B29" t="s" s="9">
         <v>59</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="10">
         <v>97489</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="10">
         <v>60000</v>
       </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" ht="12.6" customHeight="1">
-      <c r="A30" t="s" s="3">
+      <c r="A30" t="s" s="5">
         <v>60</v>
       </c>
-      <c r="B30" t="s" s="3">
+      <c r="B30" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="6">
         <v>86637</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="6">
         <v>70000</v>
       </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" ht="12.6" customHeight="1">
-      <c r="A31" t="s" s="5">
+      <c r="A31" t="s" s="9">
         <v>62</v>
       </c>
-      <c r="B31" t="s" s="5">
+      <c r="B31" t="s" s="9">
         <v>63</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="10">
         <v>124313</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="10">
         <v>50000</v>
       </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" ht="12.6" customHeight="1">
-      <c r="A32" t="s" s="3">
+      <c r="A32" t="s" s="5">
         <v>64</v>
       </c>
-      <c r="B32" t="s" s="3">
+      <c r="B32" t="s" s="5">
         <v>65</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="6">
         <v>91489</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="6">
         <v>35000</v>
       </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" ht="12.6" customHeight="1">
-      <c r="A33" t="s" s="5">
+      <c r="A33" t="s" s="9">
         <v>66</v>
       </c>
-      <c r="B33" t="s" s="5">
+      <c r="B33" t="s" s="9">
         <v>67</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="10">
         <v>140602</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="10">
         <v>25000</v>
       </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" ht="12.6" customHeight="1">
-      <c r="A34" t="s" s="3">
+      <c r="A34" t="s" s="5">
         <v>68</v>
       </c>
-      <c r="B34" t="s" s="3">
+      <c r="B34" t="s" s="5">
         <v>69</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="6">
         <v>60101</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="6">
         <v>80000</v>
       </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" ht="12.6" customHeight="1">
-      <c r="A35" t="s" s="5">
+      <c r="A35" t="s" s="9">
         <v>70</v>
       </c>
-      <c r="B35" t="s" s="5">
+      <c r="B35" t="s" s="9">
         <v>71</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="10">
         <v>141102</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="10">
         <v>15000</v>
       </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" ht="12.6" customHeight="1">
-      <c r="A36" t="s" s="3">
+      <c r="A36" t="s" s="5">
         <v>72</v>
       </c>
-      <c r="B36" t="s" s="3">
+      <c r="B36" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="6">
         <v>113898</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="6">
         <v>35000</v>
       </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" ht="12.6" customHeight="1">
-      <c r="A37" t="s" s="5">
+      <c r="A37" t="s" s="9">
         <v>74</v>
       </c>
-      <c r="B37" t="s" s="5">
+      <c r="B37" t="s" s="9">
         <v>75</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="10">
         <v>111068</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="10">
         <v>85000</v>
       </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" ht="12.6" customHeight="1">
-      <c r="A38" t="s" s="3">
+      <c r="A38" t="s" s="5">
         <v>76</v>
       </c>
-      <c r="B38" t="s" s="3">
+      <c r="B38" t="s" s="5">
         <v>77</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="6">
         <v>24287</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="6">
         <v>45000</v>
       </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" ht="12.6" customHeight="1">
-      <c r="A39" t="s" s="5">
+      <c r="A39" t="s" s="9">
         <v>78</v>
       </c>
-      <c r="B39" t="s" s="5">
+      <c r="B39" t="s" s="9">
         <v>79</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="10">
         <v>138542</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="10">
         <v>35000</v>
       </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" ht="12.6" customHeight="1">
-      <c r="A40" t="s" s="3">
+      <c r="A40" t="s" s="5">
         <v>80</v>
       </c>
-      <c r="B40" t="s" s="3">
+      <c r="B40" t="s" s="5">
         <v>81</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="6">
         <v>52436</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="6">
         <v>75000</v>
       </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" ht="12.6" customHeight="1">
-      <c r="A41" t="s" s="5">
+      <c r="A41" t="s" s="9">
         <v>82</v>
       </c>
-      <c r="B41" t="s" s="5">
+      <c r="B41" t="s" s="9">
         <v>83</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="10">
         <v>64130</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="10">
         <v>50000</v>
       </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" ht="12.6" customHeight="1">
-      <c r="A42" t="s" s="3">
+      <c r="A42" t="s" s="5">
         <v>84</v>
       </c>
-      <c r="B42" t="s" s="3">
+      <c r="B42" t="s" s="5">
         <v>85</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="6">
         <v>27872</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="6">
         <v>90000</v>
       </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" ht="12.6" customHeight="1">
-      <c r="A43" t="s" s="5">
+      <c r="A43" t="s" s="9">
         <v>86</v>
       </c>
-      <c r="B43" t="s" s="5">
+      <c r="B43" t="s" s="9">
         <v>87</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="10">
         <v>119258</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="10">
         <v>85000</v>
       </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" ht="12.6" customHeight="1">
-      <c r="A44" t="s" s="3">
+      <c r="A44" t="s" s="5">
         <v>88</v>
       </c>
-      <c r="B44" t="s" s="3">
+      <c r="B44" t="s" s="5">
         <v>89</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="6">
         <v>133576</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="6">
         <v>60000</v>
       </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" ht="12.6" customHeight="1">
-      <c r="A45" t="s" s="5">
+      <c r="A45" t="s" s="9">
         <v>90</v>
       </c>
-      <c r="B45" t="s" s="5">
+      <c r="B45" t="s" s="9">
         <v>91</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="10">
         <v>29530</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="10">
         <v>70000</v>
       </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" ht="12.6" customHeight="1">
-      <c r="A46" t="s" s="3">
+      <c r="A46" t="s" s="5">
         <v>92</v>
       </c>
-      <c r="B46" t="s" s="3">
+      <c r="B46" t="s" s="5">
         <v>93</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="6">
         <v>86186</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="6">
         <v>15000</v>
       </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" ht="12.6" customHeight="1">
-      <c r="A47" t="s" s="5">
+      <c r="A47" t="s" s="9">
         <v>94</v>
       </c>
-      <c r="B47" t="s" s="5">
+      <c r="B47" t="s" s="9">
         <v>95</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="10">
         <v>137708</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="10">
         <v>65000</v>
       </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" ht="12.6" customHeight="1">
-      <c r="A48" t="s" s="3">
+      <c r="A48" t="s" s="5">
         <v>96</v>
       </c>
-      <c r="B48" t="s" s="3">
+      <c r="B48" t="s" s="5">
         <v>97</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="6">
         <v>42450</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="6">
         <v>95000</v>
       </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" ht="12.6" customHeight="1">
-      <c r="A49" t="s" s="5">
+      <c r="A49" t="s" s="9">
         <v>98</v>
       </c>
-      <c r="B49" t="s" s="5">
+      <c r="B49" t="s" s="9">
         <v>99</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="10">
         <v>5937</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="10">
         <v>100000</v>
       </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" ht="12.6" customHeight="1">
-      <c r="A50" t="s" s="3">
+      <c r="A50" t="s" s="5">
         <v>100</v>
       </c>
-      <c r="B50" t="s" s="3">
+      <c r="B50" t="s" s="5">
         <v>101</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="6">
         <v>54805</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="6">
         <v>85000</v>
       </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51" ht="12.6" customHeight="1">
-      <c r="A51" t="s" s="5">
+      <c r="A51" t="s" s="9">
         <v>102</v>
       </c>
-      <c r="B51" t="s" s="5">
+      <c r="B51" t="s" s="9">
         <v>103</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="10">
         <v>109884</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="10">
         <v>30000</v>
       </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" ht="12.6" customHeight="1">
-      <c r="A52" t="s" s="3">
-        <v>104</v>
-      </c>
-      <c r="B52" t="s" s="3">
-        <v>105</v>
-      </c>
-      <c r="C52" s="4">
-        <v>51170</v>
-      </c>
-      <c r="D52" s="4">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="53" ht="12.6" customHeight="1">
-      <c r="A53" t="s" s="5">
-        <v>106</v>
-      </c>
-      <c r="B53" t="s" s="5">
-        <v>107</v>
-      </c>
-      <c r="C53" s="6">
-        <v>47641</v>
-      </c>
-      <c r="D53" s="6">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="54" ht="12.6" customHeight="1">
-      <c r="A54" t="s" s="3">
-        <v>108</v>
-      </c>
-      <c r="B54" t="s" s="3">
-        <v>109</v>
-      </c>
-      <c r="C54" s="4">
-        <v>7144</v>
-      </c>
-      <c r="D54" s="4">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="55" ht="12.6" customHeight="1">
-      <c r="A55" t="s" s="5">
-        <v>110</v>
-      </c>
-      <c r="B55" t="s" s="5">
-        <v>111</v>
-      </c>
-      <c r="C55" s="6">
-        <v>92559</v>
-      </c>
-      <c r="D55" s="6">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="56" ht="12.6" customHeight="1">
-      <c r="A56" t="s" s="3">
-        <v>112</v>
-      </c>
-      <c r="B56" t="s" s="3">
-        <v>113</v>
-      </c>
-      <c r="C56" s="4">
-        <v>143741</v>
-      </c>
-      <c r="D56" s="4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="57" ht="12.6" customHeight="1">
-      <c r="A57" t="s" s="5">
-        <v>114</v>
-      </c>
-      <c r="B57" t="s" s="5">
-        <v>115</v>
-      </c>
-      <c r="C57" s="6">
-        <v>81850</v>
-      </c>
-      <c r="D57" s="6">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="58" ht="12.6" customHeight="1">
-      <c r="A58" t="s" s="3">
-        <v>116</v>
-      </c>
-      <c r="B58" t="s" s="3">
-        <v>117</v>
-      </c>
-      <c r="C58" s="4">
-        <v>147955</v>
-      </c>
-      <c r="D58" s="4">
-        <v>95000</v>
-      </c>
-    </row>
-    <row r="59" ht="12.6" customHeight="1">
-      <c r="A59" t="s" s="5">
-        <v>118</v>
-      </c>
-      <c r="B59" t="s" s="5">
-        <v>119</v>
-      </c>
-      <c r="C59" s="6">
-        <v>54616</v>
-      </c>
-      <c r="D59" s="6">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="60" ht="12.6" customHeight="1">
-      <c r="A60" t="s" s="3">
-        <v>120</v>
-      </c>
-      <c r="B60" t="s" s="3">
-        <v>121</v>
-      </c>
-      <c r="C60" s="4">
-        <v>14058</v>
-      </c>
-      <c r="D60" s="4">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="61" ht="12.6" customHeight="1">
-      <c r="A61" t="s" s="5">
-        <v>122</v>
-      </c>
-      <c r="B61" t="s" s="5">
-        <v>123</v>
-      </c>
-      <c r="C61" s="6">
-        <v>142565</v>
-      </c>
-      <c r="D61" s="6">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="62" ht="12.6" customHeight="1">
-      <c r="A62" t="s" s="3">
-        <v>124</v>
-      </c>
-      <c r="B62" t="s" s="3">
-        <v>125</v>
-      </c>
-      <c r="C62" s="4">
-        <v>34340</v>
-      </c>
-      <c r="D62" s="4">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="63" ht="12.6" customHeight="1">
-      <c r="A63" t="s" s="5">
-        <v>126</v>
-      </c>
-      <c r="B63" t="s" s="5">
-        <v>127</v>
-      </c>
-      <c r="C63" s="6">
-        <v>138706</v>
-      </c>
-      <c r="D63" s="6">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="64" ht="12.6" customHeight="1">
-      <c r="A64" t="s" s="3">
-        <v>128</v>
-      </c>
-      <c r="B64" t="s" s="3">
-        <v>129</v>
-      </c>
-      <c r="C64" s="4">
-        <v>122920</v>
-      </c>
-      <c r="D64" s="4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="65" ht="12.6" customHeight="1">
-      <c r="A65" t="s" s="5">
-        <v>130</v>
-      </c>
-      <c r="B65" t="s" s="5">
-        <v>131</v>
-      </c>
-      <c r="C65" s="6">
-        <v>31232</v>
-      </c>
-      <c r="D65" s="6">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="66" ht="12.6" customHeight="1">
-      <c r="A66" t="s" s="3">
-        <v>132</v>
-      </c>
-      <c r="B66" t="s" s="3">
-        <v>133</v>
-      </c>
-      <c r="C66" s="4">
-        <v>57911</v>
-      </c>
-      <c r="D66" s="4">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="67" ht="12.6" customHeight="1">
-      <c r="A67" t="s" s="5">
-        <v>134</v>
-      </c>
-      <c r="B67" t="s" s="5">
-        <v>135</v>
-      </c>
-      <c r="C67" s="6">
-        <v>74324</v>
-      </c>
-      <c r="D67" s="6">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="68" ht="12.6" customHeight="1">
-      <c r="A68" t="s" s="3">
-        <v>136</v>
-      </c>
-      <c r="B68" t="s" s="3">
-        <v>137</v>
-      </c>
-      <c r="C68" s="4">
-        <v>68780</v>
-      </c>
-      <c r="D68" s="4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="69" ht="12.6" customHeight="1">
-      <c r="A69" t="s" s="5">
-        <v>138</v>
-      </c>
-      <c r="B69" t="s" s="5">
-        <v>139</v>
-      </c>
-      <c r="C69" s="6">
-        <v>85027</v>
-      </c>
-      <c r="D69" s="6">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="70" ht="12.6" customHeight="1">
-      <c r="A70" t="s" s="3">
-        <v>140</v>
-      </c>
-      <c r="B70" t="s" s="3">
-        <v>141</v>
-      </c>
-      <c r="C70" s="4">
-        <v>87622</v>
-      </c>
-      <c r="D70" s="4">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="71" ht="12.6" customHeight="1">
-      <c r="A71" t="s" s="5">
-        <v>142</v>
-      </c>
-      <c r="B71" t="s" s="5">
-        <v>143</v>
-      </c>
-      <c r="C71" s="6">
-        <v>83559</v>
-      </c>
-      <c r="D71" s="6">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="72" ht="12.6" customHeight="1">
-      <c r="A72" t="s" s="3">
-        <v>144</v>
-      </c>
-      <c r="B72" t="s" s="3">
-        <v>145</v>
-      </c>
-      <c r="C72" s="4">
-        <v>24997</v>
-      </c>
-      <c r="D72" s="4">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="73" ht="12.6" customHeight="1">
-      <c r="A73" t="s" s="5">
-        <v>146</v>
-      </c>
-      <c r="B73" t="s" s="5">
-        <v>147</v>
-      </c>
-      <c r="C73" s="6">
-        <v>108017</v>
-      </c>
-      <c r="D73" s="6">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="74" ht="12.6" customHeight="1">
-      <c r="A74" t="s" s="3">
-        <v>148</v>
-      </c>
-      <c r="B74" t="s" s="3">
-        <v>149</v>
-      </c>
-      <c r="C74" s="4">
-        <v>56186</v>
-      </c>
-      <c r="D74" s="4">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="75" ht="12.6" customHeight="1">
-      <c r="A75" t="s" s="5">
-        <v>150</v>
-      </c>
-      <c r="B75" t="s" s="5">
-        <v>151</v>
-      </c>
-      <c r="C75" s="6">
-        <v>36795</v>
-      </c>
-      <c r="D75" s="6">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="76" ht="12.6" customHeight="1">
-      <c r="A76" t="s" s="3">
-        <v>152</v>
-      </c>
-      <c r="B76" t="s" s="3">
-        <v>153</v>
-      </c>
-      <c r="C76" s="4">
-        <v>26638</v>
-      </c>
-      <c r="D76" s="4">
-        <v>95000</v>
-      </c>
-    </row>
-    <row r="77" ht="12.6" customHeight="1">
-      <c r="A77" t="s" s="5">
-        <v>154</v>
-      </c>
-      <c r="B77" t="s" s="5">
-        <v>155</v>
-      </c>
-      <c r="C77" s="6">
-        <v>56783</v>
-      </c>
-      <c r="D77" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="78" ht="12.6" customHeight="1">
-      <c r="A78" t="s" s="3">
-        <v>156</v>
-      </c>
-      <c r="B78" t="s" s="3">
-        <v>157</v>
-      </c>
-      <c r="C78" s="4">
-        <v>9865</v>
-      </c>
-      <c r="D78" s="4">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="79" ht="12.6" customHeight="1">
-      <c r="A79" t="s" s="5">
-        <v>158</v>
-      </c>
-      <c r="B79" t="s" s="5">
-        <v>159</v>
-      </c>
-      <c r="C79" s="6">
-        <v>63834</v>
-      </c>
-      <c r="D79" s="6">
-        <v>95000</v>
-      </c>
-    </row>
-    <row r="80" ht="12.6" customHeight="1">
-      <c r="A80" t="s" s="3">
-        <v>160</v>
-      </c>
-      <c r="B80" t="s" s="3">
-        <v>161</v>
-      </c>
-      <c r="C80" s="4">
-        <v>138272</v>
-      </c>
-      <c r="D80" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="81" ht="12.6" customHeight="1">
-      <c r="A81" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="B81" t="s" s="5">
-        <v>162</v>
-      </c>
-      <c r="C81" s="6">
-        <v>119548</v>
-      </c>
-      <c r="D81" s="6">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="82" ht="12.6" customHeight="1">
-      <c r="A82" t="s" s="3">
-        <v>163</v>
-      </c>
-      <c r="B82" t="s" s="3">
-        <v>164</v>
-      </c>
-      <c r="C82" s="4">
-        <v>88588</v>
-      </c>
-      <c r="D82" s="4">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="83" ht="12.6" customHeight="1">
-      <c r="A83" t="s" s="5">
-        <v>165</v>
-      </c>
-      <c r="B83" t="s" s="5">
-        <v>166</v>
-      </c>
-      <c r="C83" s="6">
-        <v>118401</v>
-      </c>
-      <c r="D83" s="6">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="84" ht="12.6" customHeight="1">
-      <c r="A84" t="s" s="3">
-        <v>167</v>
-      </c>
-      <c r="B84" t="s" s="3">
-        <v>168</v>
-      </c>
-      <c r="C84" s="4">
-        <v>74285</v>
-      </c>
-      <c r="D84" s="4">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="85" ht="12.6" customHeight="1">
-      <c r="A85" t="s" s="5">
-        <v>169</v>
-      </c>
-      <c r="B85" t="s" s="5">
-        <v>170</v>
-      </c>
-      <c r="C85" s="6">
-        <v>143057</v>
-      </c>
-      <c r="D85" s="6">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="86" ht="12.6" customHeight="1">
-      <c r="A86" t="s" s="3">
-        <v>171</v>
-      </c>
-      <c r="B86" t="s" s="3">
-        <v>172</v>
-      </c>
-      <c r="C86" s="4">
-        <v>6538</v>
-      </c>
-      <c r="D86" s="4">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="87" ht="12.6" customHeight="1">
-      <c r="A87" t="s" s="5">
-        <v>173</v>
-      </c>
-      <c r="B87" t="s" s="5">
-        <v>174</v>
-      </c>
-      <c r="C87" s="6">
-        <v>95073</v>
-      </c>
-      <c r="D87" s="6">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="88" ht="12.6" customHeight="1">
-      <c r="A88" t="s" s="3">
-        <v>175</v>
-      </c>
-      <c r="B88" t="s" s="3">
-        <v>176</v>
-      </c>
-      <c r="C88" s="4">
-        <v>130018</v>
-      </c>
-      <c r="D88" s="4">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="89" ht="12.6" customHeight="1">
-      <c r="A89" t="s" s="5">
-        <v>177</v>
-      </c>
-      <c r="B89" t="s" s="5">
-        <v>178</v>
-      </c>
-      <c r="C89" s="6">
-        <v>140718</v>
-      </c>
-      <c r="D89" s="6">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="90" ht="12.6" customHeight="1">
-      <c r="A90" t="s" s="3">
-        <v>179</v>
-      </c>
-      <c r="B90" t="s" s="3">
-        <v>180</v>
-      </c>
-      <c r="C90" s="4">
-        <v>92045</v>
-      </c>
-      <c r="D90" s="4">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="91" ht="12.6" customHeight="1">
-      <c r="A91" t="s" s="5">
-        <v>181</v>
-      </c>
-      <c r="B91" t="s" s="5">
-        <v>182</v>
-      </c>
-      <c r="C91" s="6">
-        <v>72145</v>
-      </c>
-      <c r="D91" s="6">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="92" ht="12.6" customHeight="1">
-      <c r="A92" t="s" s="3">
-        <v>183</v>
-      </c>
-      <c r="B92" t="s" s="3">
-        <v>184</v>
-      </c>
-      <c r="C92" s="4">
-        <v>17243</v>
-      </c>
-      <c r="D92" s="4">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="93" ht="12.6" customHeight="1">
-      <c r="A93" t="s" s="5">
-        <v>185</v>
-      </c>
-      <c r="B93" t="s" s="5">
-        <v>186</v>
-      </c>
-      <c r="C93" s="6">
-        <v>112338</v>
-      </c>
-      <c r="D93" s="6">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="94" ht="12.6" customHeight="1">
-      <c r="A94" t="s" s="3">
-        <v>187</v>
-      </c>
-      <c r="B94" t="s" s="3">
-        <v>188</v>
-      </c>
-      <c r="C94" s="4">
-        <v>51569</v>
-      </c>
-      <c r="D94" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="95" ht="12.6" customHeight="1">
-      <c r="A95" t="s" s="5">
-        <v>189</v>
-      </c>
-      <c r="B95" t="s" s="5">
-        <v>190</v>
-      </c>
-      <c r="C95" s="6">
-        <v>105337</v>
-      </c>
-      <c r="D95" s="6">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="96" ht="12.6" customHeight="1">
-      <c r="A96" t="s" s="3">
-        <v>191</v>
-      </c>
-      <c r="B96" t="s" s="3">
-        <v>192</v>
-      </c>
-      <c r="C96" s="4">
-        <v>63310</v>
-      </c>
-      <c r="D96" s="4">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="97" ht="12.6" customHeight="1">
-      <c r="A97" t="s" s="5">
-        <v>193</v>
-      </c>
-      <c r="B97" t="s" s="5">
-        <v>194</v>
-      </c>
-      <c r="C97" s="6">
-        <v>119671</v>
-      </c>
-      <c r="D97" s="6">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="98" ht="12.6" customHeight="1">
-      <c r="A98" t="s" s="3">
-        <v>195</v>
-      </c>
-      <c r="B98" t="s" s="3">
-        <v>196</v>
-      </c>
-      <c r="C98" s="4">
-        <v>66958</v>
-      </c>
-      <c r="D98" s="4">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="99" ht="12.6" customHeight="1">
-      <c r="A99" t="s" s="5">
-        <v>197</v>
-      </c>
-      <c r="B99" t="s" s="5">
-        <v>198</v>
-      </c>
-      <c r="C99" s="6">
-        <v>145487</v>
-      </c>
-      <c r="D99" s="6">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="100" ht="12.6" customHeight="1">
-      <c r="A100" t="s" s="3">
-        <v>199</v>
-      </c>
-      <c r="B100" t="s" s="3">
-        <v>200</v>
-      </c>
-      <c r="C100" s="4">
-        <v>24549</v>
-      </c>
-      <c r="D100" s="4">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="101" ht="12.6" customHeight="1">
-      <c r="A101" t="s" s="5">
-        <v>201</v>
-      </c>
-      <c r="B101" t="s" s="5">
-        <v>202</v>
-      </c>
-      <c r="C101" s="6">
-        <v>50451</v>
-      </c>
-      <c r="D101" s="6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="102" ht="12.6" customHeight="1">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3378,6 +2447,5 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>